<commit_message>
Creación de departamento con cuentas
</commit_message>
<xml_diff>
--- a/PlanCuentas.xlsx
+++ b/PlanCuentas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual\Proyecto_Roberto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95302781-3489-4382-8076-02CFCA191BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD526563-7102-4DD4-8FFE-266DB8E75E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A3F66D12-4FCB-48B9-8EDE-634F8DB9845A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$206</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1581,10 +1581,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8E9AF1-4AC8-4155-A90E-2D1A2E1E696A}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1604,7 +1605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1626,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1637,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1758,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1846,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1934,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1956,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1978,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1989,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -2011,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -2044,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -2066,7 +2067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2099,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>103</v>
       </c>
@@ -2176,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -2198,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -2220,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -2242,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -2253,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -2286,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -2297,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>126</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -2330,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -2352,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2396,7 +2397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -2418,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -2451,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -2484,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -2495,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -2506,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -2528,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -2561,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -2583,7 +2584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>189</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>191</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>193</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>195</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>197</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>199</v>
       </c>
@@ -2715,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>200</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>202</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>204</v>
       </c>
@@ -2748,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>206</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>208</v>
       </c>
@@ -2770,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>210</v>
       </c>
@@ -2781,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>212</v>
       </c>
@@ -2792,7 +2793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>214</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>216</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>218</v>
       </c>
@@ -2825,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>219</v>
       </c>
@@ -2836,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>221</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>222</v>
       </c>
@@ -2858,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>224</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>226</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>228</v>
       </c>
@@ -2891,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>230</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>231</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>233</v>
       </c>
@@ -2924,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>235</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>237</v>
       </c>
@@ -2946,7 +2947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>239</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>241</v>
       </c>
@@ -2968,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>243</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>244</v>
       </c>
@@ -2990,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>246</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>247</v>
       </c>
@@ -3012,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>249</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>251</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>253</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>255</v>
       </c>
@@ -3056,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>257</v>
       </c>
@@ -3067,7 +3068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>259</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>261</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>263</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>265</v>
       </c>
@@ -3111,7 +3112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>267</v>
       </c>
@@ -3122,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>269</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>270</v>
       </c>
@@ -3144,7 +3145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>271</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>273</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>275</v>
       </c>
@@ -3177,7 +3178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>277</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>279</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>281</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>283</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>285</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>287</v>
       </c>
@@ -3243,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>289</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>291</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>293</v>
       </c>
@@ -3276,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>295</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>297</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>299</v>
       </c>
@@ -3309,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>301</v>
       </c>
@@ -3320,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>303</v>
       </c>
@@ -3331,7 +3332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>305</v>
       </c>
@@ -3342,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>307</v>
       </c>
@@ -3353,7 +3354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>309</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>311</v>
       </c>
@@ -3375,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>313</v>
       </c>
@@ -3386,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>315</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>317</v>
       </c>
@@ -3408,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>319</v>
       </c>
@@ -3419,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>321</v>
       </c>
@@ -3430,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>323</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>325</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>327</v>
       </c>
@@ -3463,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>329</v>
       </c>
@@ -3474,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>331</v>
       </c>
@@ -3485,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>333</v>
       </c>
@@ -3496,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>335</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>337</v>
       </c>
@@ -3518,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>339</v>
       </c>
@@ -3529,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>341</v>
       </c>
@@ -3540,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>343</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>345</v>
       </c>
@@ -3562,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>347</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>349</v>
       </c>
@@ -3584,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>351</v>
       </c>
@@ -3595,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>352</v>
       </c>
@@ -3606,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>353</v>
       </c>
@@ -3617,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>355</v>
       </c>
@@ -3628,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>357</v>
       </c>
@@ -3639,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>359</v>
       </c>
@@ -3650,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>361</v>
       </c>
@@ -3661,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>362</v>
       </c>
@@ -3672,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>364</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>366</v>
       </c>
@@ -3694,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>368</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>370</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>372</v>
       </c>
@@ -3727,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>373</v>
       </c>
@@ -3738,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>374</v>
       </c>
@@ -3749,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>375</v>
       </c>
@@ -3760,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>377</v>
       </c>
@@ -3771,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>379</v>
       </c>
@@ -3782,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>381</v>
       </c>
@@ -3793,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>383</v>
       </c>
@@ -3804,7 +3805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>385</v>
       </c>
@@ -3815,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>387</v>
       </c>
@@ -3826,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>389</v>
       </c>
@@ -3837,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>391</v>
       </c>
@@ -3848,7 +3849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>393</v>
       </c>
@@ -3860,7 +3861,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{6D8E9AF1-4AC8-4155-A90E-2D1A2E1E696A}"/>
+  <autoFilter ref="A1:C206" xr:uid="{6D8E9AF1-4AC8-4155-A90E-2D1A2E1E696A}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="CTAS POR COBRAR"/>
+        <filter val="Ctas.por Cobrar Clientes"/>
+        <filter val="CTAS.POR COBRAR EMPLEADOS"/>
+        <filter val="CUENTAS POR COBRAR IMPUESTOS"/>
+        <filter val="OTRAS CUENTAS POR COBRAR"/>
+        <filter val="Otras cuentas por cobrar (Alm)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>